<commit_message>
Player finance specs update
</commit_message>
<xml_diff>
--- a/Design/FlowchartExcel.xlsx
+++ b/Design/FlowchartExcel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="360" windowWidth="27795" windowHeight="14130" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="360" windowWidth="27795" windowHeight="14130" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="GUI FLOW" sheetId="2" r:id="rId1"/>
@@ -13033,7 +13033,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fi-FI" sz="1100"/>
-            <a:t>-1400</a:t>
+            <a:t>-2400</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -13090,7 +13090,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fi-FI" sz="1100"/>
-            <a:t>-2900</a:t>
+            <a:t>-1900</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -13336,7 +13336,7 @@
     <xdr:to>
       <xdr:col>64</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -13347,7 +13347,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12629029" y="190500"/>
-          <a:ext cx="3866030" cy="2095500"/>
+          <a:ext cx="3866030" cy="2476500"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -14768,16 +14768,766 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fi-FI" sz="1100"/>
-            <a:t>DEBT</a:t>
+            <a:t>PLAYER</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
-            <a:t> 1 PAYMENT</a:t>
+            <a:t> MONEY</a:t>
           </a:r>
           <a:endParaRPr lang="fi-FI" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3092824" y="5715000"/>
+          <a:ext cx="3092823" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>COMMENT:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>DEBT 1 PAYMENT = MONTHLY CUT + INTEREST</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>22413</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Elbow Connector 3"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="40" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="2549340" y="3882838"/>
+          <a:ext cx="3429000" cy="235323"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="515471" y="5715000"/>
+          <a:ext cx="2061882" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>COMMENT:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>PLAYER MONEY = amount</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> of money the player has at the given moment</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Elbow Connector 9"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="1"/>
+          <a:endCxn id="108" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="515471" y="1524000"/>
+          <a:ext cx="12700" cy="4667250"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1800000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6443382" y="5715000"/>
+          <a:ext cx="2061883" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>COMMENT:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>PAYMENT</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> TOTAL = sum of all DEBT PAYMENTS</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Elbow Connector 12"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="11" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="4846545" y="3087220"/>
+          <a:ext cx="1905000" cy="3350559"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rectangle 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3092824" y="6858000"/>
+          <a:ext cx="2061882" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>COMMENT:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>EXISTING</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> CASH = PLAYER MONEY - PAYMENT TOTAL</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Elbow Connector 17"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="15" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="2835088" y="4762500"/>
+          <a:ext cx="257736" cy="2476500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Rectangle 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8763000" y="5715000"/>
+          <a:ext cx="1804147" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>COMMENT:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>Incremental change = 100</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Elbow Connector 22"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="106" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="7972986" y="4151779"/>
+          <a:ext cx="2095500" cy="1030941"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>257734</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>128868</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Elbow Connector 24"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="77" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="8530478" y="3291728"/>
+          <a:ext cx="3429000" cy="1417545"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Rectangle 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11340353" y="5715000"/>
+          <a:ext cx="1804147" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>COMMENT:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>MONTHLY</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> CUT = 1000;</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Elbow Connector 30"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="95" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="9177618" y="2521323"/>
+          <a:ext cx="3810000" cy="2577353"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -19225,8 +19975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BO35" sqref="BO35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BA25" sqref="BA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19256,7 +20006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AL21" sqref="AL21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Shadows for all + Temp tile cleanup
</commit_message>
<xml_diff>
--- a/Design/FlowchartExcel.xlsx
+++ b/Design/FlowchartExcel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="420" windowWidth="27795" windowHeight="14070" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="420" windowWidth="27795" windowHeight="14070" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="GUI FLOW" sheetId="2" r:id="rId1"/>
@@ -16907,11 +16907,11 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fi-FI" sz="1100"/>
-            <a:t>Lights -</a:t>
+            <a:t>Lights </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
-            <a:t> Top Floor (on/off)</a:t>
+            <a:t>(on/off)</a:t>
           </a:r>
           <a:endParaRPr lang="fi-FI" sz="1100"/>
         </a:p>
@@ -16934,7 +16934,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 10"/>
+        <xdr:cNvPr id="12" name="Rectangle 11"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -16969,63 +16969,6 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fi-FI" sz="1100"/>
-            <a:t>Lights - Bottom Floor (on/off)</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Rectangle 11"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1028701" y="4572000"/>
-          <a:ext cx="1543050" cy="571500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="fi-FI" sz="1100"/>
             <a:t>Elevator</a:t>
           </a:r>
           <a:r>
@@ -17040,68 +16983,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Rectangle 12"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1028701" y="5143500"/>
-          <a:ext cx="1543050" cy="571500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="fi-FI" sz="1100"/>
-            <a:t>Weapon system power</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
-            <a:t> (on/off)</a:t>
-          </a:r>
-          <a:endParaRPr lang="fi-FI" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>31</xdr:row>
@@ -17348,7 +17229,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="Rectangle 19"/>
+        <xdr:cNvPr id="21" name="Rectangle 20"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17383,8 +17264,13 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fi-FI" sz="1100"/>
-            <a:t>Weapon systems (on/off)</a:t>
-          </a:r>
+            <a:t>Automated</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> Defences (on/off)</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -17405,7 +17291,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Rectangle 20"/>
+        <xdr:cNvPr id="22" name="Rectangle 21"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17440,68 +17326,6 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fi-FI" sz="1100"/>
-            <a:t>Automated</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
-            <a:t> Defences (on/off)</a:t>
-          </a:r>
-          <a:endParaRPr lang="fi-FI" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Rectangle 21"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7715250" y="3810000"/>
-          <a:ext cx="1800225" cy="571500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="fi-FI" sz="1100"/>
             <a:t>Open</a:t>
           </a:r>
           <a:r>
@@ -17518,13 +17342,13 @@
     <xdr:from>
       <xdr:col>30</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -17534,7 +17358,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7715250" y="4572000"/>
+          <a:off x="7715250" y="3810000"/>
           <a:ext cx="1800225" cy="571500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -19393,7 +19217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BB26" sqref="BB26"/>
     </sheetView>
   </sheetViews>
@@ -20648,8 +20472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AL21" sqref="AL21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finance specs update (excel)
</commit_message>
<xml_diff>
--- a/Design/FlowchartExcel.xlsx
+++ b/Design/FlowchartExcel.xlsx
@@ -15419,13 +15419,13 @@
     <xdr:from>
       <xdr:col>44</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -15435,7 +15435,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11340353" y="5715000"/>
+          <a:off x="11340353" y="6096000"/>
           <a:ext cx="1804147" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15492,22 +15492,23 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>48</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>128868</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="31" name="Elbow Connector 30"/>
         <xdr:cNvCxnSpPr>
+          <a:stCxn id="26" idx="0"/>
           <a:endCxn id="95" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="9177618" y="2521323"/>
-          <a:ext cx="3810000" cy="2577353"/>
+          <a:off x="8922684" y="2776257"/>
+          <a:ext cx="4191000" cy="2448486"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -15543,7 +15544,7 @@
     <xdr:to>
       <xdr:col>64</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -15554,7 +15555,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12629029" y="2857500"/>
-          <a:ext cx="3866030" cy="2667000"/>
+          <a:ext cx="3866030" cy="3048000"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -15661,6 +15662,17 @@
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
+          <a:endParaRPr lang="fi-FI" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t>So interest would be 10% for the first month, 15% for the second month, and so on.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
           <a:endParaRPr lang="fi-FI" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -15671,13 +15683,13 @@
     <xdr:from>
       <xdr:col>44</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -15687,7 +15699,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11340353" y="6477000"/>
+          <a:off x="11340353" y="6858000"/>
           <a:ext cx="1804147" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -20886,7 +20898,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BN33" sqref="BN33"/>
+      <selection activeCell="BT22" sqref="BT22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Look at my Excel, my Excel is amazing! Give it a lick. "Mmm, it tastes just like raisins"
</commit_message>
<xml_diff>
--- a/Design/FlowchartExcel.xlsx
+++ b/Design/FlowchartExcel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="27795" windowHeight="14010" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="540" windowWidth="27795" windowHeight="13950" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="GUI FLOW" sheetId="2" r:id="rId1"/>
@@ -13100,63 +13100,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="Rectangle 51"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1800225" y="11239500"/>
-          <a:ext cx="1800225" cy="381000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="fi-FI" sz="1100"/>
-            <a:t>TOTAL</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
@@ -17854,6 +17797,1040 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="771525" y="7429500"/>
+          <a:ext cx="6429375" cy="2476500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2571749" y="7620000"/>
+          <a:ext cx="2571751" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>CONSOLE BÖÖ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rectangle 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4371975" y="6096000"/>
+          <a:ext cx="1285875" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Rectangle 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028700" y="8181975"/>
+          <a:ext cx="1285875" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>BASIC</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> ACTION 1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Rectangle 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028700" y="8572500"/>
+          <a:ext cx="1285875" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>BASIC</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> ACTION 2</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Rectangle 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028700" y="8953500"/>
+          <a:ext cx="1285875" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>ACTION</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> REQUIRES HACKING 1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Rectangle 26"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2314575" y="8953500"/>
+          <a:ext cx="771525" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>HACKING</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> ICON</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="Rectangle 27"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="771525" y="10477500"/>
+          <a:ext cx="3600450" cy="2095500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>ACCESS</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> DENIED</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fi-FI" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t>Security Level: very low / low / med / high / very high</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t>Your hacking rate: n</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t>Chance of success: n%</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Rectangle 28"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028700" y="12001500"/>
+          <a:ext cx="1285875" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>HACK</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Rectangle 29"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2571750" y="12001500"/>
+          <a:ext cx="1285875" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>CANCEL</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>128588</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Elbow Connector 30"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="26" idx="2"/>
+          <a:endCxn id="28" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1645444" y="9551194"/>
+          <a:ext cx="952500" cy="900112"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Rectangle 32"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6943725" y="10477500"/>
+          <a:ext cx="3600450" cy="2095500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>ACCESS DENIED</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fi-FI" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t>Your internal systems have been damaged.</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Rectangle 33"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4886325" y="11239500"/>
+          <a:ext cx="1285875" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>IF FAIL</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Arrow Connector 35"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="28" idx="3"/>
+          <a:endCxn id="33" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4371975" y="11525250"/>
+          <a:ext cx="2571750" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="Rectangle 36"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1285875" y="12954000"/>
+          <a:ext cx="1285875" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>IF SUCCESS</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Rectangle 37"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="771525" y="13716000"/>
+          <a:ext cx="3600450" cy="2095500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>ACCESS GRANTED</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fi-FI" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t>&lt;what ever is supposed to happen, happens&gt;</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Straight Arrow Connector 39"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="28" idx="2"/>
+          <a:endCxn id="38" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2571750" y="12573000"/>
+          <a:ext cx="0" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -20897,8 +21874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BT22" sqref="BT22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BV16" sqref="BV16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20928,8 +21905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="S73" sqref="S73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>